<commit_message>
Info update 11 May, 2018
</commit_message>
<xml_diff>
--- a/Thedal/resource/TestCase/Thedal_Automation_Testcase.xlsx
+++ b/Thedal/resource/TestCase/Thedal_Automation_Testcase.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13035"/>
+    <workbookView windowWidth="28695" windowHeight="13035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
+    <sheet name="Actions" sheetId="2" r:id="rId2"/>
+    <sheet name="Pages" sheetId="4" r:id="rId3"/>
+    <sheet name="Locator" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147">
   <si>
     <t>Test Description</t>
   </si>
@@ -146,6 +149,315 @@
   </si>
   <si>
     <t>C:\Users\Knila5\Pictures\download1.jpg</t>
+  </si>
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Use to click on the element</t>
+  </si>
+  <si>
+    <t>Use to Enter inside the element</t>
+  </si>
+  <si>
+    <t>EnterAndTab</t>
+  </si>
+  <si>
+    <t>Use to Enter inside the element and Press tab key</t>
+  </si>
+  <si>
+    <t>Clear the content inside the textbox and Enter inside the element</t>
+  </si>
+  <si>
+    <t>ClearEnterTab</t>
+  </si>
+  <si>
+    <t>Clear the content inside the textbox and Enter inside the element and Press tab key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used to navigate to any URL </t>
+  </si>
+  <si>
+    <t>Choose</t>
+  </si>
+  <si>
+    <t>Choose any value from Dropdown field</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Select any value from Dropdown field</t>
+  </si>
+  <si>
+    <t>VerifyPageTitle</t>
+  </si>
+  <si>
+    <t>Used to verify the title of a page</t>
+  </si>
+  <si>
+    <t>Used to Read/Verify the Content inside a field/label</t>
+  </si>
+  <si>
+    <t>VerifyElementPresent</t>
+  </si>
+  <si>
+    <t>Used to verify/Check the element isVisible/isDisabled</t>
+  </si>
+  <si>
+    <t>Used to upload any image file to FileUploadControl Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actions </t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Steps - Mandatory,</t>
+  </si>
+  <si>
+    <t>Action - Mandatory,</t>
+  </si>
+  <si>
+    <t>ElementType - Mandatory,</t>
+  </si>
+  <si>
+    <t>ElementPath - Mandatory,</t>
+  </si>
+  <si>
+    <t>value - Optional</t>
+  </si>
+  <si>
+    <t>value - Mandatory</t>
+  </si>
+  <si>
+    <t>Action - Optional,</t>
+  </si>
+  <si>
+    <t>ElementType - Optional,</t>
+  </si>
+  <si>
+    <t>ElementPath - Optional,</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>Textbox</t>
+  </si>
+  <si>
+    <t>txtbx</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>DropDown/Combo</t>
+  </si>
+  <si>
+    <t>drpdwn</t>
+  </si>
+  <si>
+    <t>ForgetPassword</t>
+  </si>
+  <si>
+    <t>forgetfassword</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>ResetPassword</t>
+  </si>
+  <si>
+    <t>resetpassword</t>
+  </si>
+  <si>
+    <t>RadioButton</t>
+  </si>
+  <si>
+    <t>rdbtn</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>CheckBox</t>
+  </si>
+  <si>
+    <t>ckbx</t>
+  </si>
+  <si>
+    <t>AdminList</t>
+  </si>
+  <si>
+    <t>adminlist</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>btn</t>
+  </si>
+  <si>
+    <t>AddAdmin</t>
+  </si>
+  <si>
+    <t>addadmin</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>lnk</t>
+  </si>
+  <si>
+    <t>EditAdmin</t>
+  </si>
+  <si>
+    <t>editadmin</t>
+  </si>
+  <si>
+    <t>CityAdminList</t>
+  </si>
+  <si>
+    <t>cityadminlist</t>
+  </si>
+  <si>
+    <t>AddCityAdmin</t>
+  </si>
+  <si>
+    <t>addcityadmin</t>
+  </si>
+  <si>
+    <t>EditCityAdmin</t>
+  </si>
+  <si>
+    <t>editcityadmin</t>
+  </si>
+  <si>
+    <t>SupervisorList</t>
+  </si>
+  <si>
+    <t>supervisorlist</t>
+  </si>
+  <si>
+    <t>AddSupervisor</t>
+  </si>
+  <si>
+    <t>addsupervisor</t>
+  </si>
+  <si>
+    <t>EditSupervisor</t>
+  </si>
+  <si>
+    <t>editsupervisor</t>
+  </si>
+  <si>
+    <t>VendorList</t>
+  </si>
+  <si>
+    <t>vendorlist</t>
+  </si>
+  <si>
+    <t>AddVendor</t>
+  </si>
+  <si>
+    <t>addvendor</t>
+  </si>
+  <si>
+    <t>EditVendor</t>
+  </si>
+  <si>
+    <t>editvendor</t>
+  </si>
+  <si>
+    <t>AddUserList</t>
+  </si>
+  <si>
+    <t>adduserlist</t>
+  </si>
+  <si>
+    <t>AddVolunteer</t>
+  </si>
+  <si>
+    <t>addvolunteer</t>
+  </si>
+  <si>
+    <t>AddBloodDonor</t>
+  </si>
+  <si>
+    <t>addblooddonor</t>
+  </si>
+  <si>
+    <t>CityList</t>
+  </si>
+  <si>
+    <t>citylist</t>
+  </si>
+  <si>
+    <t>AddCity</t>
+  </si>
+  <si>
+    <t>addcity</t>
+  </si>
+  <si>
+    <t>EditCity</t>
+  </si>
+  <si>
+    <t>editcity</t>
+  </si>
+  <si>
+    <t>ThedalVideoList</t>
+  </si>
+  <si>
+    <t>thedalvideolist</t>
+  </si>
+  <si>
+    <t>AddThedalVideo</t>
+  </si>
+  <si>
+    <t>addthedalvideo</t>
+  </si>
+  <si>
+    <t>EditThedalVideo</t>
+  </si>
+  <si>
+    <t>editthedalvideo</t>
+  </si>
+  <si>
+    <t>ElementName</t>
+  </si>
+  <si>
+    <t>ElementID</t>
+  </si>
+  <si>
+    <t>ElementLocation</t>
   </si>
 </sst>
 </file>
@@ -158,10 +470,18 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -184,14 +504,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,7 +631,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,25 +640,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,169 +830,28 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -616,7 +957,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -634,144 +975,171 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1095,8 +1463,8 @@
   <sheetPr/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1141,7 +1509,7 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1158,7 +1526,7 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1194,7 +1562,7 @@
       <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="12" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1225,7 +1593,7 @@
       <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1233,8 +1601,8 @@
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
@@ -1249,7 +1617,7 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="10" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1357,4 +1725,1190 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K87"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="77.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="14.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="14.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="6">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="6">
+        <v>3</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="6">
+        <v>4</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="6">
+        <v>5</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="6">
+        <v>6</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="6">
+        <v>7</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="6">
+        <v>8</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="6">
+        <v>9</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="6"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="6">
+        <v>10</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="6"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="6">
+        <v>11</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C76" s="6"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="6">
+        <v>12</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C82" s="6"/>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A40:A45"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="A64:A69"/>
+    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="A76:A81"/>
+    <mergeCell ref="A82:A87"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="B46:B51"/>
+    <mergeCell ref="B52:B57"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="B64:B69"/>
+    <mergeCell ref="B70:B75"/>
+    <mergeCell ref="B76:B81"/>
+    <mergeCell ref="B82:B87"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="12.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="11.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="17.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="18.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="3">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6">
+      <c r="D9" s="3">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6">
+      <c r="D10" s="3">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6">
+      <c r="D11" s="3">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6">
+      <c r="D12" s="3">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6">
+      <c r="D13" s="3">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6">
+      <c r="D14" s="3">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6">
+      <c r="D15" s="3">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6">
+      <c r="D16" s="3">
+        <v>15</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6">
+      <c r="D17" s="3">
+        <v>16</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6">
+      <c r="D18" s="3">
+        <v>17</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
+      <c r="D19" s="3">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6">
+      <c r="D20" s="3">
+        <v>19</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6">
+      <c r="D21" s="3">
+        <v>20</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6">
+      <c r="D22" s="3">
+        <v>21</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6">
+      <c r="D23" s="3">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6">
+      <c r="D24" s="3">
+        <v>23</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6">
+      <c r="D25" s="3">
+        <v>24</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6">
+      <c r="D26" s="3">
+        <v>25</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="2" max="2" width="18.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="13.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>